<commit_message>
Updated 3D print files, monocular display software instructions
</commit_message>
<xml_diff>
--- a/Hardware/Parts Lists.xlsx
+++ b/Hardware/Parts Lists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\misaa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\misaa\Documents\GitHub\mouseVRheadset\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED708A12-2A69-4EFB-8F3C-24561A030051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2831A8-D284-412B-BA5E-8EC2477A1C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2364" yWindow="3492" windowWidth="20304" windowHeight="12696" activeTab="1" xr2:uid="{1EFD0954-5A5A-4050-8BE3-B1038B12A517}"/>
+    <workbookView xWindow="2364" yWindow="3492" windowWidth="20304" windowHeight="12696" xr2:uid="{1EFD0954-5A5A-4050-8BE3-B1038B12A517}"/>
   </bookViews>
   <sheets>
     <sheet name="Binocular headset" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="95">
   <si>
     <t>link</t>
   </si>
@@ -183,12 +183,6 @@
     <t>MouseEyepieceBack_V3.stl</t>
   </si>
   <si>
-    <t>RaspberryPiCaseBack_V3.stl</t>
-  </si>
-  <si>
-    <t>RaspberryPiCaseFront_V3.stl</t>
-  </si>
-  <si>
     <t>MouseEyepieceFront_V3.stl</t>
   </si>
   <si>
@@ -211,9 +205,6 @@
   </si>
   <si>
     <t>Teensy40</t>
-  </si>
-  <si>
-    <t>Black tape</t>
   </si>
   <si>
     <t>https://www.thorlabs.com/thorproduct.cfm?partnumber=T137-1.0</t>
@@ -283,6 +274,66 @@
   </si>
   <si>
     <t>see README for 3D printing instructions</t>
+  </si>
+  <si>
+    <t>lens holder</t>
+  </si>
+  <si>
+    <t>display holder</t>
+  </si>
+  <si>
+    <t>DisplayHolder_V1.stl</t>
+  </si>
+  <si>
+    <t>LensHolder_V1.stl</t>
+  </si>
+  <si>
+    <t>RaspberryPiCaseFront_V4.stl</t>
+  </si>
+  <si>
+    <t>RaspberryPiCaseBack_V4.stl</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/4261A37/</t>
+  </si>
+  <si>
+    <t>4261A37</t>
+  </si>
+  <si>
+    <t>Needle File, Tapered Rectangular, for Extra Fine Finish</t>
+  </si>
+  <si>
+    <t>(suggested) Needle file</t>
+  </si>
+  <si>
+    <t>(suggested) super glue</t>
+  </si>
+  <si>
+    <t>Instant-Bond Adhesive, Loctite® 495, 0.1 FL. oz. Tube</t>
+  </si>
+  <si>
+    <t>7520A13</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/7520A13/</t>
+  </si>
+  <si>
+    <t>(suggested) silicone glue</t>
+  </si>
+  <si>
+    <t>Silicone Sealant, Dow Corning 732, 3 FL. oz. Tube</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/7587A2/</t>
+  </si>
+  <si>
+    <t>7587A2</t>
+  </si>
+  <si>
+    <t>(suggested) black tape</t>
+  </si>
+  <si>
+    <t>~$&lt;5 + shipping</t>
   </si>
 </sst>
 </file>
@@ -325,15 +376,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
+      <b/>
+      <sz val="13.5"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -377,9 +429,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -390,8 +439,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -707,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AED3B4-0086-434F-B10A-10628E1341B6}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,27 +779,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:6" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>1</v>
       </c>
     </row>
@@ -759,7 +813,7 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -779,7 +833,7 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -799,7 +853,7 @@
       <c r="C5" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -819,7 +873,7 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -839,10 +893,10 @@
       <c r="C7" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>0.27</v>
       </c>
       <c r="F7" s="1">
@@ -851,17 +905,17 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C8"/>
-      <c r="D8" s="8" t="s">
-        <v>60</v>
+      <c r="D8" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
@@ -877,10 +931,10 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>20.27</v>
       </c>
       <c r="F9" s="1">
@@ -889,19 +943,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="6">
-        <v>10.95</v>
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4295</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="5">
+        <v>45</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
@@ -909,19 +963,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
       </c>
       <c r="C11" s="1">
-        <v>4295</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="6">
-        <v>45</v>
+        <v>1322</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="5">
+        <v>8.9499999999999993</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
@@ -935,13 +989,13 @@
         <v>65</v>
       </c>
       <c r="C12" s="1">
-        <v>1322</v>
-      </c>
-      <c r="D12" s="5" t="s">
+        <v>4298</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="6">
-        <v>8.9499999999999993</v>
+      <c r="E12" s="5">
+        <v>7.95</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
@@ -949,19 +1003,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C13" s="1">
-        <v>4298</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="6">
-        <v>7.95</v>
+        <v>2693</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="5">
+        <v>19.95</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
@@ -969,97 +1023,193 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="5">
+        <v>19.170000000000002</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="5">
+        <v>5.29</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="5">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="5">
+        <v>10.95</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B18"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="8"/>
+    </row>
+    <row r="20" spans="1:6" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="1">
-        <v>2693</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="E21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="6">
-        <v>19.95</v>
-      </c>
-      <c r="F14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A17" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="7" t="s">
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" s="1">
         <v>2</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="8" t="s">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F20" s="1">
-        <v>1</v>
+      <c r="C24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1068,22 +1218,23 @@
     <hyperlink ref="D3" r:id="rId2" xr:uid="{F9EC1067-5577-47EB-94B5-8C14A6D3F0B3}"/>
     <hyperlink ref="D6" r:id="rId3" xr:uid="{182A7565-0CF9-412A-8350-A8427069F5FB}"/>
     <hyperlink ref="D9" r:id="rId4" xr:uid="{85179E83-B483-49A9-BCB2-55B63FF49EFF}"/>
-    <hyperlink ref="D11" r:id="rId5" xr:uid="{CC664B47-D8A7-4398-99C5-284200295F22}"/>
+    <hyperlink ref="D10" r:id="rId5" xr:uid="{CC664B47-D8A7-4398-99C5-284200295F22}"/>
     <hyperlink ref="D5" r:id="rId6" xr:uid="{2C5D62FB-5A23-4ECF-B665-47C256933A2F}"/>
-    <hyperlink ref="D13" r:id="rId7" xr:uid="{DD2A698E-F559-478D-AE55-F5BA81626346}"/>
-    <hyperlink ref="D12" r:id="rId8" xr:uid="{580EC65A-ACBA-47B4-9529-2510CA5D0A44}"/>
+    <hyperlink ref="D12" r:id="rId7" xr:uid="{DD2A698E-F559-478D-AE55-F5BA81626346}"/>
+    <hyperlink ref="D11" r:id="rId8" xr:uid="{580EC65A-ACBA-47B4-9529-2510CA5D0A44}"/>
     <hyperlink ref="D7" r:id="rId9" xr:uid="{AF61F227-4E64-467B-B112-3356CF757AFC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9FBA31F-62F5-4DC0-9EF6-9E66E4CAFB1B}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1098,27 +1249,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:6" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1132,7 +1283,7 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -1152,7 +1303,7 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -1172,7 +1323,7 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -1192,10 +1343,10 @@
       <c r="C6" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>0.27</v>
       </c>
       <c r="F6" s="1">
@@ -1204,17 +1355,17 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7"/>
-      <c r="D7" s="8" t="s">
-        <v>60</v>
+      <c r="D7" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -1230,10 +1381,10 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>20.27</v>
       </c>
       <c r="F8" s="1">
@@ -1242,19 +1393,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="6">
-        <v>10.95</v>
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="5">
+        <v>23.8</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
@@ -1262,96 +1413,190 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="5">
+        <v>19.170000000000002</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="5">
+        <v>5.29</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="5">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="6">
-        <v>23.8</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A13" s="2" t="s">
+      <c r="E13" s="5">
+        <v>10.95</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
+    <row r="16" spans="1:6" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="7" t="s">
+      <c r="C16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="E16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="8" t="s">
+      <c r="C17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="1">
+      <c r="C20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed innacuracy in gdshader; Added Pi header to parts list
</commit_message>
<xml_diff>
--- a/Hardware/Parts Lists.xlsx
+++ b/Hardware/Parts Lists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\misaa\Documents\GitHub\mouseVRheadset\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2831A8-D284-412B-BA5E-8EC2477A1C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE308F26-D020-4D5D-9C75-BCD2905901C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2364" yWindow="3492" windowWidth="20304" windowHeight="12696" xr2:uid="{1EFD0954-5A5A-4050-8BE3-B1038B12A517}"/>
+    <workbookView xWindow="2112" yWindow="4548" windowWidth="24552" windowHeight="12696" xr2:uid="{1EFD0954-5A5A-4050-8BE3-B1038B12A517}"/>
   </bookViews>
   <sheets>
     <sheet name="Binocular headset" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="97">
   <si>
     <t>link</t>
   </si>
@@ -334,6 +334,12 @@
   </si>
   <si>
     <t>~$&lt;5 + shipping</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/2222</t>
+  </si>
+  <si>
+    <t>GPIO Header for Raspberry Pi A+/B+/Pi 2/Pi 3/Pi 4/Zero - 2x20 Female Header</t>
   </si>
 </sst>
 </file>
@@ -443,7 +449,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -761,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AED3B4-0086-434F-B10A-10628E1341B6}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1022,20 +1028,17 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C14" t="s">
-        <v>82</v>
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2222</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="E14" s="5">
-        <v>19.170000000000002</v>
+        <v>1.5</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
@@ -1043,19 +1046,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E15" s="5">
-        <v>5.29</v>
+        <v>19.170000000000002</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
@@ -1063,19 +1066,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E16" s="5">
-        <v>8.9600000000000009</v>
+        <v>5.29</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
@@ -1083,81 +1086,81 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" s="5">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>58</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E18" s="5">
         <v>10.95</v>
       </c>
-      <c r="F17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B18"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A19" s="2" t="s">
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B19"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="8"/>
-    </row>
-    <row r="20" spans="1:6" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
+      <c r="B20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B21" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="1">
+      <c r="F21" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>67</v>
@@ -1174,10 +1177,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>67</v>
@@ -1186,18 +1189,18 @@
         <v>74</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F23" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>67</v>
@@ -1209,6 +1212,26 @@
         <v>94</v>
       </c>
       <c r="F24" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added files for small form factor headset
</commit_message>
<xml_diff>
--- a/Hardware/Parts Lists.xlsx
+++ b/Hardware/Parts Lists.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\misaa\Documents\GitHub\mouseVRheadset\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C968DC0-3665-487D-8DCF-88DDEE71F5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0CD328-0728-4800-B83E-F977B241AA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1704" yWindow="4188" windowWidth="24552" windowHeight="12696" xr2:uid="{1EFD0954-5A5A-4050-8BE3-B1038B12A517}"/>
+    <workbookView xWindow="1836" yWindow="4632" windowWidth="24552" windowHeight="12696" activeTab="1" xr2:uid="{1EFD0954-5A5A-4050-8BE3-B1038B12A517}"/>
   </bookViews>
   <sheets>
     <sheet name="Binocular headset" sheetId="2" r:id="rId1"/>
     <sheet name="Monocular eyepiece" sheetId="1" r:id="rId2"/>
+    <sheet name="Small form factor headset" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="112">
   <si>
     <t>link</t>
   </si>
@@ -337,6 +338,42 @@
   </si>
   <si>
     <t>Fresnel lens</t>
+  </si>
+  <si>
+    <t>RaspyGC9307_minibrdV1_2023-07-01</t>
+  </si>
+  <si>
+    <t>RaspyGC9307_minihatV1_2023-07-01</t>
+  </si>
+  <si>
+    <t>miniHeadet_V1.stl</t>
+  </si>
+  <si>
+    <t>headet enclosure</t>
+  </si>
+  <si>
+    <t>PZN-12-VV</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/omnetics/A79622-001/15784989?s=N4IgTCBcDaIA4C8B2BaAjGFA3LIC6AvkA</t>
+  </si>
+  <si>
+    <t>SPI cable connector</t>
+  </si>
+  <si>
+    <t>omnetics polarized nano connector, 12 position, surface mount, vertical smt (VV)</t>
+  </si>
+  <si>
+    <t>SPI cable</t>
+  </si>
+  <si>
+    <t>RHD SPI Interface cable (various lengths available, standard or ultrathin, example is standard 3 ft)</t>
+  </si>
+  <si>
+    <t>C3203</t>
+  </si>
+  <si>
+    <t>https://intantech.com/RHD_SPI_cables.html</t>
   </si>
 </sst>
 </file>
@@ -766,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AED3B4-0086-434F-B10A-10628E1341B6}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1256,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9FBA31F-62F5-4DC0-9EF6-9E66E4CAFB1B}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1651,4 +1688,531 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0D6476-A293-471A-9A2D-A487858AAF12}">
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21" style="1" customWidth="1"/>
+    <col min="2" max="2" width="86.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.27</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="5">
+        <v>58.81</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" s="5">
+        <v>215</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10"/>
+      <c r="D10" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="5">
+        <v>20.27</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="1">
+        <v>4295</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="5">
+        <v>45</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1322</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="5">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4298</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="5">
+        <v>7.95</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2693</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="5">
+        <v>19.95</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2222</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="5">
+        <v>19.170000000000002</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="5">
+        <v>5.29</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="5">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="1">
+        <v>10411739</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="5">
+        <v>3.29</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B22"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{B90E0979-86B8-4F16-BA2F-CEEC90FAA203}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{09A140CB-C77A-4ECB-A4B1-2623246596AF}"/>
+    <hyperlink ref="D12" r:id="rId3" xr:uid="{47C26D90-49E7-42AD-9F56-FFF24E39488D}"/>
+    <hyperlink ref="D13" r:id="rId4" xr:uid="{B4039E43-22D9-4B6F-AED2-82F50F6A602E}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{9EBFFC64-5851-4C8A-B473-15026E9ED4AE}"/>
+    <hyperlink ref="D15" r:id="rId6" xr:uid="{B1A92D5C-7D5F-4B6B-AFCE-1C28A5F2E506}"/>
+    <hyperlink ref="D14" r:id="rId7" xr:uid="{8AFE7D81-FE04-4D7E-B591-C9C5AE425C82}"/>
+    <hyperlink ref="D7" r:id="rId8" xr:uid="{2497F740-709B-4AB0-A76C-E1103CA2CDCD}"/>
+    <hyperlink ref="D3" r:id="rId9" xr:uid="{7E100F74-CEEE-43E2-B8C8-FA6C9BB59DD6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated small form factor headset 3D prints
</commit_message>
<xml_diff>
--- a/Hardware/Parts Lists.xlsx
+++ b/Hardware/Parts Lists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\misaa\Documents\GitHub\mouseVRheadset\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0CD328-0728-4800-B83E-F977B241AA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AA9C97-7D87-4508-B5FB-D099C091481A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1836" yWindow="4632" windowWidth="24552" windowHeight="12696" activeTab="1" xr2:uid="{1EFD0954-5A5A-4050-8BE3-B1038B12A517}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="27288" windowHeight="17544" activeTab="2" xr2:uid="{1EFD0954-5A5A-4050-8BE3-B1038B12A517}"/>
   </bookViews>
   <sheets>
     <sheet name="Binocular headset" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="114">
   <si>
     <t>link</t>
   </si>
@@ -346,12 +346,6 @@
     <t>RaspyGC9307_minihatV1_2023-07-01</t>
   </si>
   <si>
-    <t>miniHeadet_V1.stl</t>
-  </si>
-  <si>
-    <t>headet enclosure</t>
-  </si>
-  <si>
     <t>PZN-12-VV</t>
   </si>
   <si>
@@ -374,6 +368,18 @@
   </si>
   <si>
     <t>https://intantech.com/RHD_SPI_cables.html</t>
+  </si>
+  <si>
+    <t>miniHeadset_V2_backing.stl</t>
+  </si>
+  <si>
+    <t>headset enclosure back</t>
+  </si>
+  <si>
+    <t>headset eyepiece</t>
+  </si>
+  <si>
+    <t>miniHeadset_V2_eyepiece.stl</t>
   </si>
 </sst>
 </file>
@@ -1293,7 +1299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9FBA31F-62F5-4DC0-9EF6-9E66E4CAFB1B}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -1692,10 +1698,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0D6476-A293-471A-9A2D-A487858AAF12}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1836,16 +1842,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E8" s="5">
         <v>58.81</v>
@@ -1856,16 +1862,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" t="s">
         <v>108</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="C9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="E9" s="5">
         <v>215</v>
@@ -2143,10 +2149,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>62</v>
@@ -2163,10 +2169,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>62</v>
@@ -2175,7 +2181,7 @@
         <v>69</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="F26" s="1">
         <v>2</v>
@@ -2183,10 +2189,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>62</v>
@@ -2198,6 +2204,26 @@
         <v>88</v>
       </c>
       <c r="F27" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>